<commit_message>
updated documentation and blender file
</commit_message>
<xml_diff>
--- a/fdm/stl/filesandsettings.xlsx
+++ b/fdm/stl/filesandsettings.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\kinetic-display\fdm\stl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92EE89E-315C-4718-97B5-024383900A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A44F93-7C68-4EBE-AACB-125E750A290B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="228" windowWidth="17280" windowHeight="10308" xr2:uid="{D0B1DBA1-9AFF-44C2-A8AD-2E890C375429}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D0B1DBA1-9AFF-44C2-A8AD-2E890C375429}"/>
   </bookViews>
   <sheets>
     <sheet name="FDM" sheetId="1" r:id="rId1"/>
-    <sheet name="BOM" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="BOM" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="107">
   <si>
     <t>Layer Height</t>
   </si>
@@ -262,6 +263,102 @@
   </si>
   <si>
     <t>Segment rack gear (use TPU setting)</t>
+  </si>
+  <si>
+    <t>28 AWG Gauge Flexible Silicone Rubber Electric Wire 6 Colors 32.8 feet each</t>
+  </si>
+  <si>
+    <t>A4 Size Felt Sheets with Adhesive Backing, Peel and Stick Felt Sheets Adhesive Backed, Felt Adhesive Sheet</t>
+  </si>
+  <si>
+    <t>Digital Temperature and Humidity Sensor DHT11 LED Module,Blue</t>
+  </si>
+  <si>
+    <t>5mm 0.5 Ω ohm Photoresistor LDR Resistor 5516 GL5516 Light-Dependent Photoconductor (Photo Light Sensitive)</t>
+  </si>
+  <si>
+    <t>M2 x 8mm Stainless Steel Phillips Round Head Self Tapping Screws</t>
+  </si>
+  <si>
+    <t>M2 x 6mm Stainless Steel Phillips Round Head Self Tapping Screws</t>
+  </si>
+  <si>
+    <t>M2 X 15mm Stainless Steel Phillips Round Head Self Tapping Screws</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Micro 130 DC Motor Strong Magnetic Brushed Electric DC 3V -12V 25000 RPM Cars Toys Electric Motor, High Speed Torque DIY Remote Control Toy Car Hobby Motor, Metal Car Engine Motor Kit for Toys</t>
+  </si>
+  <si>
+    <t>5mm Flat Top LED Diode Lights (Clear Transparent Lens) Bright Lighting Bulb Lamps Electronics Components Indicator Light Emitting Diodes</t>
+  </si>
+  <si>
+    <t>3mm Flat Top LED Diode Lights (Clear Transparent Lens) Bright Lighting Bulb Lamps Electronics Components Indicator Light Emitting Diodes</t>
+  </si>
+  <si>
+    <t>Vertical Slide Switches Micro High Knob 3 Pin 2 Position 1P2T SPDT Panel Mount AC 125V 2A</t>
+  </si>
+  <si>
+    <t>2 Inch Jumbo Paper Clips (Smooth Big Paperclips)</t>
+  </si>
+  <si>
+    <t>Dupont Jumper Wire Cable Female Pin Connector 2.54mm</t>
+  </si>
+  <si>
+    <t>2.54mm 1x2p Dupont Connector Housing Female for Dupont Cable and Jumper Wire</t>
+  </si>
+  <si>
+    <t>2.54mm 0.1" Pitch PCB Mount Screw Terminal Block Connector, 2P 3P 4P Terminals 150V 6A for 26-18AWG Cable</t>
+  </si>
+  <si>
+    <t>LM2596 DC-DC Step Down Variable Volt Regulator Input 3.2V-40V Output 1.25V-35V Adjustable Buck Converter Electronic Voltage Stabilizer Power Supply Module</t>
+  </si>
+  <si>
+    <t>2.1mm Barrel Jack 5.5x2.1mm Female DC Power Jack 2.1 X 5.5mm DC Jack Connector 6V 9V 12V DC Jack Panel Mount</t>
+  </si>
+  <si>
+    <t>12V 5A Power Supply, Waysse Power Supply Adapter, AC DC Converter 100-220V to 12 Volt 5 Amp Transformer 5.5x2.1mm Plug</t>
+  </si>
+  <si>
+    <t>S8050D S8050 NPN Transistor TO-92 20V 700MA 1W</t>
+  </si>
+  <si>
+    <t>1N4001 Diode, standard, 1A, 50V, DO-41</t>
+  </si>
+  <si>
+    <t>SONGLE SRS-05VDC-SL 05VDC-SL 4100 Blue 5V 6PIN Power Relay Original</t>
+  </si>
+  <si>
+    <t>L293D 16-pin IC Stepper Motor Drivers Controller</t>
+  </si>
+  <si>
+    <t>0.1uF Ceramic Disc Capacitor - 50 Volts</t>
+  </si>
+  <si>
+    <t>1uF Electrolytic Capacitor 1UF-50V-5X11</t>
+  </si>
+  <si>
+    <t>SS8550 TO-92 PNP Transistor</t>
+  </si>
+  <si>
+    <t>2N2222 TO-92 - NPN Transistor</t>
+  </si>
+  <si>
+    <t>10K ohm Resistor 1/2w (0.5Watt) ±1% Tolerance Metal Film Fixed Resistor</t>
+  </si>
+  <si>
+    <t>Vertical Slide Switch Micro High Knob 3 Pin 2 Position 1P2T SPDT Panel Mount AC 125V 2A</t>
+  </si>
+  <si>
+    <t>Raspberry pi 2040 pico</t>
+  </si>
+  <si>
+    <t>Raspberry pi 2040 pico-W</t>
+  </si>
+  <si>
+    <t>(optional) 20pin x 10pcs Female Headers Pins Straight Single Row Gold Plated Pitch 2.54mm 0.1 inch for PCB Connector Machine Breadboard Electronic Circuit Board</t>
   </si>
 </sst>
 </file>
@@ -297,9 +394,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01392322-4639-4FE3-9D84-6BEF39AEE8A4}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1680,15 +1795,468 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1DBA57-A32D-46BC-82BF-67A2F33BAC20}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EEBFD5-29AC-4ADB-8C3F-BE9339A7072F}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2">
+        <f>B7*B8</f>
+        <v>39</v>
+      </c>
+      <c r="C9" s="2">
+        <f>C7*C8</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1DBA57-A32D-46BC-82BF-67A2F33BAC20}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection sqref="A1:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="55.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="2">
+        <f>4*28</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="2">
+        <f>4*3+5</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added images and documentation
</commit_message>
<xml_diff>
--- a/fdm/stl/filesandsettings.xlsx
+++ b/fdm/stl/filesandsettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\kinetic-display\fdm\stl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332DA80A-38C3-4A4D-AA4A-7EA98F19AE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01380BBA-55F2-4D81-8EDB-C32123A54B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0B1DBA1-9AFF-44C2-A8AD-2E890C375429}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="108">
   <si>
     <t>Layer Height</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Segment rack gear</t>
+  </si>
+  <si>
+    <t>Yes (10%)</t>
   </si>
 </sst>
 </file>
@@ -752,7 +755,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P21"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,7 +1277,7 @@
         <v>21</v>
       </c>
       <c r="O10" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="P10" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
fixed bug in json around the 56 minute mark
</commit_message>
<xml_diff>
--- a/fdm/stl/filesandsettings.xlsx
+++ b/fdm/stl/filesandsettings.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\kinetic-display\fdm\stl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01380BBA-55F2-4D81-8EDB-C32123A54B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55E2724-5CD8-4376-A348-75E7375FCCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0B1DBA1-9AFF-44C2-A8AD-2E890C375429}"/>
   </bookViews>
   <sheets>
     <sheet name="FDM" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="BOM" sheetId="2" r:id="rId3"/>
+    <sheet name="BOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -265,9 +264,6 @@
     <t>A4 Size Felt Sheets with Adhesive Backing, Peel and Stick Felt Sheets Adhesive Backed, Felt Adhesive Sheet</t>
   </si>
   <si>
-    <t>Digital Temperature and Humidity Sensor DHT11 LED Module,Blue</t>
-  </si>
-  <si>
     <t>5mm 0.5 Ω ohm Photoresistor LDR Resistor 5516 GL5516 Light-Dependent Photoconductor (Photo Light Sensitive)</t>
   </si>
   <si>
@@ -362,6 +358,9 @@
   </si>
   <si>
     <t>Yes (10%)</t>
+  </si>
+  <si>
+    <t>Digital Temperature and Humidity Sensor DHT22 Module</t>
   </si>
 </sst>
 </file>
@@ -397,17 +396,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -755,7 +748,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,7 +1179,7 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>72</v>
@@ -1277,7 +1270,7 @@
         <v>21</v>
       </c>
       <c r="O10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P10" t="s">
         <v>43</v>
@@ -1288,7 +1281,7 @@
         <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
         <v>72</v>
@@ -1798,54 +1791,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EEBFD5-29AC-4ADB-8C3F-BE9339A7072F}">
-  <dimension ref="A13:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" style="2" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1DBA57-A32D-46BC-82BF-67A2F33BAC20}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection sqref="A1:B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="8.88671875" style="7"/>
+    <col min="3" max="3" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B2" s="2">
@@ -1853,38 +1822,38 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>85</v>
+      <c r="A3" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
     <row r="7" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>81</v>
+      <c r="A7" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B7" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B8" s="2">
@@ -1892,40 +1861,40 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>86</v>
+      <c r="A9" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B9" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>87</v>
+      <c r="A10" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B10" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>82</v>
+      <c r="A13" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B13" s="2">
         <f>4*28</f>
@@ -1933,88 +1902,88 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>83</v>
+      <c r="A14" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>84</v>
+      <c r="A15" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="B17" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>104</v>
+      <c r="A22" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B22" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="B24" s="2">
         <f>4*3+5</f>
@@ -2022,64 +1991,64 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>96</v>
+      <c r="A25" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B25" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>97</v>
+      <c r="A26" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="B26" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="B29" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="B31" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>103</v>
+      <c r="A32" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>

</xml_diff>